<commit_message>
Few updates with prognosis plot etc.
</commit_message>
<xml_diff>
--- a/spring_flod_analysis.xlsx
+++ b/spring_flod_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\personalfolders\u39545_Sarah\EtteranalyseLTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E7BBFB-465C-4FC4-9554-3836A3CDF3C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBF420F-A35E-4D4D-99B0-00A95C1AE11D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18006" windowHeight="6699" xr2:uid="{EB861DC1-2A69-4366-9E6B-67ADF5EDEFAB}"/>
   </bookViews>
@@ -1152,7 +1152,7 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>174928</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="16554616" cy="12351651"/>
+    <xdr:ext cx="13071943" cy="22513022"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1">
@@ -1167,7 +1167,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="548641" y="174928"/>
-          <a:ext cx="16554616" cy="12351651"/>
+          <a:ext cx="13071943" cy="22513022"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1211,7 +1211,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="nb-NO" sz="1100" baseline="0"/>
-            <a:t> is a guide to how to use the jupyter/pyhon method to do the annual spring flod analysis. There are a few steps that needs to be done before going into the script i jupyter.</a:t>
+            <a:t> is a thorough guide to how to use the Jupyter script spring_flod_analysis.ipynp together with this document to do the annual spring flod analysis. I will also guide you throug a few initial steps that needs to be done to get started.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1219,70 +1219,20 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="nb-NO" sz="1100" baseline="0"/>
-            <a:t>1. Check that all snow updates have been registrated in this document under the sheets: Snow updates, Norg-Reg1, ..., Norg-Reg8, Sver-Reg1, ..., Sver-Reg4.</a:t>
+            <a:rPr lang="nb-NO" sz="1100" b="1" baseline="0"/>
+            <a:t>BACKGROUND INFO</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="nb-NO" sz="1100" baseline="0"/>
-            <a:t>2. Now thats done you should note yourself the last week that there was updates in the first round (spring time), and from that figure out the very last date any snow updates </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="nb-NO" sz="1100" baseline="0"/>
-            <a:t>lead to a new </a:t>
-          </a:r>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
           <a:r>
             <a:rPr lang="nb-NO" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>snow status</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="nb-NO" sz="1100" baseline="0"/>
-            <a:t>. Then noe the day after that last status down in the sheet: save abat runs i the column B2 (TEMP).</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="nb-NO" sz="1100" baseline="0"/>
-            <a:t>3. Figure out what date toy want the reference model to start from, and write it in the same sheet as above and in the column B3 (REF).</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="nb-NO" sz="1100" baseline="0"/>
-            <a:t>4. Well done so far. Now it is time to run Abat:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="nb-NO" sz="1100" baseline="0"/>
-            <a:t>First of all you need to update the different models in Abat: LTM, REF and TEMP. We also need to figure out from what date </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="nb-NO" sz="1100" b="0" i="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1291,7 +1241,124 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>First you need to run the Abat job for HBV_Oppdatering_TEMP, but do this after</a:t>
+            <a:t>There is three models that we use to analyse the spring flood: LTM, REF, TEMP. LTM is the operative model, and it includes both snow and temperature adjustments. REF is the samen model but it is not updated with any adjustemnts. TEMP is likeLTM but it does not include temperature adjustments. There is actually one more model called SNOW, and that one does not include snow adjustments, but we don't use that here.</a:t>
+          </a:r>
+          <a:endParaRPr lang="nb-NO">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" b="1" baseline="0"/>
+            <a:t>INITIAL STEPS</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" baseline="0"/>
+            <a:t>-&gt; Its a good idea to start with checking that all snow updates have been registrated in this document under the sheets: Norg-Reg1, ..., Norg-Reg8, Sver-Reg1, ..., Sver-Reg4. Here you should write for excample u09 if the update happened between tuesday (after prognosis delivered) in week nine and tuesday (before prognosis delivered) week ten. In the sheet </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Snow updates you should give each week, e.eg. u09, were done a specific color. This is done so that the delivered prognosis (p.50) before and after each snow update can be plotted. Another reason for doing this is so that we have an overview of all snow updates which we will need in the next step.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>-&gt; Figure out when to start REF from. I will call this date "REF date" form now on You should also figure out the very last date any snow updates lead to a new snow status ideally before the melting starts. I will call this date "TEMP date" form now on. Now write down those times in the sheet: "save abat runs" in column B2 (TEMP) and B3 (REF). There might be snow updates done later at the end of the melting season i.e. to delete snow, but we separates the two types of snow updates.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>RUNNING MODELS IN ABAT + SAVING RESULTS WITH JUPYTER</a:t>
+          </a:r>
+          <a:endParaRPr lang="nb-NO" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>-&gt; We now need</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> to run the three models LTM, TEMP and REF in Abat both to update the models if there has been any changes in the input history and to specify what we will analyse. The way we do this is by changing the start date in the specific jobs properties, before running the job. </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="nb-NO" sz="1100" b="0" i="0" baseline="0">
@@ -1303,7 +1370,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> noon (12:00)</a:t>
+            <a:t>Inside Abat you find the jobs here:</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="nb-NO" sz="1100" b="0" i="0">
@@ -1315,12 +1382,28 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>:</a:t>
+            <a:t> Jobs, Folders &amp; Plans -&gt; SMGOSL Norway -&gt; HBV -&gt; ClimateLTM.</a:t>
           </a:r>
-        </a:p>
-        <a:p>
+          <a:endParaRPr lang="nb-NO">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
           <a:r>
-            <a:rPr lang="nb-NO" sz="1100" b="0" i="0">
+            <a:rPr lang="nb-NO" sz="1100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1329,12 +1412,277 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>1. Open Abat and the server currently in use.</a:t>
+            <a:t>1. Example changing the job properties:</a:t>
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
           <a:r>
-            <a:rPr lang="nb-NO" sz="1100" b="0" i="0">
+            <a:rPr lang="nb-NO" sz="1100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1343,12 +1691,313 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>2. Then go through: Jobs, Folders &amp; Plans -&gt; SMGOSL Norway -&gt; HBV -&gt; ClimateLTM</a:t>
+            <a:t>2. Example running the job:</a:t>
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
           <a:r>
-            <a:rPr lang="nb-NO" sz="1100" b="0" i="0">
+            <a:rPr lang="nb-NO" sz="1100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1357,12 +2006,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>3. Right click on HBV-Oppdatering_TEMP and choose Properties.</a:t>
+            <a:t>-&gt; </a:t>
           </a:r>
-        </a:p>
-        <a:p>
           <a:r>
-            <a:rPr lang="nb-NO" sz="1100" b="0" i="0">
+            <a:rPr lang="nb-NO" sz="1100" b="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1371,12 +2018,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>4. Then choose Job Properties. Here you need to change the start date in Parameters, for example to:</a:t>
+            <a:t>THE NEXT STEPS SHOULD BE DONE AFTER 12:00, AND DONT STOP THE PROCESS UNTIL DONE</a:t>
           </a:r>
-        </a:p>
-        <a:p>
           <a:r>
-            <a:rPr lang="nb-NO" sz="1100" b="0" i="0" baseline="0">
+            <a:rPr lang="nb-NO" sz="1100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1385,10 +2030,61 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>     </a:t>
+            <a:t>. The process takes about two-three hours.</a:t>
           </a:r>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
           <a:r>
-            <a:rPr lang="nb-NO" sz="1100" b="0" i="0">
+            <a:rPr lang="nb-NO" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1. Now start with updating the LTM model in case of historical changes in the input. I did this by running it from 01.09 the year before and than the first of each month after that until "now" = day-1 day. But then I had 	checked that there har not been more than one snow update in one month. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>?. Q_OBSE also?</a:t>
+          </a:r>
+          <a:endParaRPr lang="nb-NO" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1397,23 +2093,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>\InflowScriptDebug\InflowRunTasks.wsf ${ICC_PATH}\ArbPktIntegrator\HBV\Climate-LTM-Oppdatering\TEMP 01.04.2018 day</a:t>
+            <a:t>2. Do the same thing</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="nb-NO" sz="1100" b="0" i="0">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
           <a:r>
-            <a:rPr lang="nb-NO" sz="1100" b="0" i="0">
+            <a:rPr lang="nb-NO" sz="1100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1422,12 +2105,13 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Don't leave because you need to change back to the original after you run the job.</a:t>
+            <a:t> for TEMP until the month of the chosen TEMP date. Then run the TEMP model from that TEMP date.</a:t>
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
           <a:r>
-            <a:rPr lang="nb-NO" sz="1100" b="0" i="0">
+            <a:rPr lang="nb-NO" sz="1100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1436,12 +2120,13 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Trigger the job manually. You can do this any time, but its okay to double check with f.eks Atle.</a:t>
+            <a:t>3. Write down the original start of the REF, and run the REF model from the chosen REF date. </a:t>
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
           <a:r>
-            <a:rPr lang="nb-NO" sz="1100" b="0" i="0">
+            <a:rPr lang="nb-NO" sz="1100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1450,12 +2135,13 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Now that the Temp models are updated in SMG we need to save them, by running this script: Cell -&gt; Run All. wait for it to print 'done'.</a:t>
+            <a:t>4. Now that both TEMP and REF is run from TEMP date and REF date we want to save the results so that we can change the properties back afterwards:</a:t>
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
           <a:r>
-            <a:rPr lang="nb-NO" sz="1100" b="0" i="0">
+            <a:rPr lang="nb-NO" sz="1100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1464,15 +2150,66 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Finally you need to change the Parameters back, and run again to :</a:t>
+            <a:t>	-&gt; Open the script </a:t>
           </a:r>
-        </a:p>
-        <a:p>
           <a:r>
-            <a:rPr lang="nb-NO"/>
-            <a:t>\InflowScriptDebug\InflowRunTasks.wsf ${ICC_PATH}\ArbPktIntegrator\HBV\Climate-LTM-Oppdatering\TEMP day-1 day</a:t>
+            <a:rPr lang="nb-NO" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>save_abat_runs.ipynp</a:t>
           </a:r>
-          <a:endParaRPr lang="nb-NO" sz="1100"/>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>, press Cell -&gt; Run All. Wait for it to print "done". Then that is done. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>5. Continue running TEMP from the first of each month until "now" = day-1 day.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>6. Change back REF to the original date (which you wrote down) in properties and run it.</a:t>
+          </a:r>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="nb-NO" sz="1100" baseline="0"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="nb-NO" sz="1100"/>
@@ -1607,6 +2344,182 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>15904</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>15902</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>277895</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>159026</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A087CF4-EF48-4FB4-9351-EE0A5EA78FF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="652008" y="4977516"/>
+          <a:ext cx="2806409" cy="3387256"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>318054</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>153611</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>413469</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>19250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20766117-078C-4E8D-9E58-09FDB7C8CF3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4134680" y="4924394"/>
+          <a:ext cx="5184250" cy="3491433"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>612253</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>122712</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>373713</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>130379</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBC78057-F5B3-491E-846B-E7E8D7CF9359}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="612253" y="9664277"/>
+          <a:ext cx="3578086" cy="1725149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>453227</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>103367</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>97982</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>7953</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C84FCFF-7114-43E0-AEC5-585690C8E54B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4905957" y="8690776"/>
+          <a:ext cx="3461382" cy="4102874"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1909,7 +2822,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13FBB199-619B-4E2F-A5AA-4F0D0622527E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="AA80" sqref="AA80"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -6943,9 +7858,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7107,26 +8025,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17C3FE88-FD63-422B-A211-481C065C3BEF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9BC95A6-9D68-4876-B344-5C0E9EA310F9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a1bb4200-479c-4a05-afd7-28ce53bfa9b9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7150,9 +8057,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9BC95A6-9D68-4876-B344-5C0E9EA310F9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17C3FE88-FD63-422B-A211-481C065C3BEF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="a1bb4200-479c-4a05-afd7-28ce53bfa9b9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Saved down new abat runs + updated method. Fixed x-axis in plots along date to show weeks/months/year.
</commit_message>
<xml_diff>
--- a/spring_flod_analysis.xlsx
+++ b/spring_flod_analysis.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\personalfolders\MEHO\spring-flod-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CBA5E1-6562-461B-95AB-9FD69EFBAAE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F7C8F3-0F75-424A-AAE3-230DEA1849D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18006" windowHeight="6699" firstSheet="10" activeTab="12" xr2:uid="{EB861DC1-2A69-4366-9E6B-67ADF5EDEFAB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18006" windowHeight="6699" tabRatio="860" firstSheet="1" activeTab="1" xr2:uid="{EB861DC1-2A69-4366-9E6B-67ADF5EDEFAB}"/>
   </bookViews>
   <sheets>
     <sheet name="user manual" sheetId="26" r:id="rId1"/>
-    <sheet name="save abat runs" sheetId="10" r:id="rId2"/>
+    <sheet name="saved abat runs" sheetId="10" r:id="rId2"/>
     <sheet name="LTM1" sheetId="1" r:id="rId3"/>
     <sheet name="LTM2" sheetId="2" r:id="rId4"/>
     <sheet name="LTM3" sheetId="3" r:id="rId5"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="320">
   <si>
     <t>Område:</t>
   </si>
@@ -810,9 +810,6 @@
     <t>Bjøl-Bjølvo........-D9100S3BT0108</t>
   </si>
   <si>
-    <t>Vikf-Hove..........-D9100S3BT0108</t>
-  </si>
-  <si>
     <t>Jost-Jostedal......-D9100S3BT0108</t>
   </si>
   <si>
@@ -822,9 +819,6 @@
     <t>Vikf-Maalset.......-D9100S3BT0108</t>
   </si>
   <si>
-    <t>Vikf-Refsdal.......-D9100S3BT0108</t>
-  </si>
-  <si>
     <t>Aura-Aura..........-D9100S3BT0108</t>
   </si>
   <si>
@@ -999,20 +993,35 @@
     <t>violet</t>
   </si>
   <si>
-    <t>TEMP</t>
-  </si>
-  <si>
-    <t>REF</t>
-  </si>
-  <si>
     <t>04.04 gjør at vi får med snøoppdatering bl.a. for jogla og tingvatn i LTM2</t>
+  </si>
+  <si>
+    <t>TEMP1</t>
+  </si>
+  <si>
+    <t>REF1</t>
+  </si>
+  <si>
+    <t>TEMP2</t>
+  </si>
+  <si>
+    <t>TEMP day-1d day</t>
+  </si>
+  <si>
+    <t>Vikf-Refsdal.......-D1050S3BT0108</t>
+  </si>
+  <si>
+    <t>Helge: Mistet antagelig en del tilsig i perioden det var nedtappet i muravatn (mai), så skulle tro Q_N_FB overestimerer, men det gjør den ikke.  Antakelig ikke snakk om så mye volum. men ingen volumendring i magasinet i denne perioden ihvertfall.</t>
+  </si>
+  <si>
+    <t>Snømålin:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1059,6 +1068,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1097,7 +1112,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -1122,6 +1137,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3542,6 +3560,106 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>151075</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>79514</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1619226" cy="609013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D387E7B-EC0F-49A8-8AC9-247EC320A01A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7999012" y="333956"/>
+          <a:ext cx="1619226" cy="609013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:alpha val="19000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln cmpd="dbl">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ORIGINALER:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" b="1"/>
+            <a:t>TEMP: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" b="0"/>
+            <a:t>TEMP day-1d day</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" b="1"/>
+            <a:t>REF:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100"/>
+            <a:t>REF 01.01.2019 day </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3900,7 +4018,7 @@
       <c r="C2" s="9"/>
       <c r="D2" s="5"/>
       <c r="E2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F2" s="6"/>
     </row>
@@ -3910,7 +4028,7 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.2" x14ac:dyDescent="0.35">
@@ -4043,7 +4161,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -4079,7 +4197,9 @@
       <c r="A2" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B2" s="9"/>
+      <c r="B2" s="9">
+        <v>43556</v>
+      </c>
       <c r="C2" s="9"/>
       <c r="D2" s="5"/>
       <c r="F2" s="6"/>
@@ -4148,6 +4268,9 @@
     <row r="13" spans="1:6" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>190</v>
+      </c>
+      <c r="B13" s="9">
+        <v>43539</v>
       </c>
       <c r="D13" s="5"/>
     </row>
@@ -4275,7 +4398,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -4322,7 +4445,9 @@
       <c r="A3" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="9">
+        <v>43511</v>
+      </c>
       <c r="C3" s="9"/>
       <c r="D3" s="5"/>
       <c r="F3" s="6"/>
@@ -4331,6 +4456,9 @@
       <c r="A4" s="2" t="s">
         <v>239</v>
       </c>
+      <c r="B4" s="9">
+        <v>43511</v>
+      </c>
       <c r="D4" s="5"/>
       <c r="F4" s="6"/>
     </row>
@@ -4358,12 +4486,18 @@
       <c r="A7" s="2" t="s">
         <v>242</v>
       </c>
+      <c r="B7" s="9">
+        <v>43525</v>
+      </c>
       <c r="D7" s="5"/>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>243</v>
+      </c>
+      <c r="B8" s="9">
+        <v>43525</v>
       </c>
       <c r="D8" s="5"/>
       <c r="F8" s="6"/>
@@ -4397,7 +4531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A39B053-7732-4ADC-8F84-B4966898327B}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -4477,7 +4611,7 @@
       </c>
       <c r="D6" s="5"/>
       <c r="F6" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -4490,7 +4624,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -4502,75 +4636,75 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B9" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -4583,7 +4717,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -4594,113 +4728,135 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>273</v>
+      <c r="D1" s="7" t="s">
+        <v>319</v>
       </c>
       <c r="F1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>83</v>
       </c>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>97</v>
       </c>
+      <c r="D3" s="5" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>84</v>
       </c>
+      <c r="D4" s="5" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>297</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>86</v>
       </c>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>88</v>
       </c>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>98</v>
       </c>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>89</v>
       </c>
       <c r="C9" t="s">
-        <v>294</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>90</v>
       </c>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>91</v>
       </c>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>92</v>
       </c>
       <c r="C12" t="s">
-        <v>294</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>93</v>
       </c>
       <c r="C13" t="s">
-        <v>296</v>
-      </c>
+        <v>294</v>
+      </c>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>94</v>
       </c>
       <c r="C14" t="s">
-        <v>294</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>96</v>
       </c>
       <c r="B15" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C15" t="s">
-        <v>294</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>111</v>
       </c>
+      <c r="D16" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4712,7 +4868,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -4723,13 +4879,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>271</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
@@ -4787,7 +4943,7 @@
         <v>110</v>
       </c>
       <c r="B12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -4830,7 +4986,7 @@
         <v>129</v>
       </c>
       <c r="B20" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -4843,7 +4999,7 @@
         <v>131</v>
       </c>
       <c r="B22" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -4856,15 +5012,15 @@
         <v>118</v>
       </c>
       <c r="B24" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B25" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -4872,7 +5028,7 @@
         <v>119</v>
       </c>
       <c r="B26" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -4880,7 +5036,7 @@
         <v>120</v>
       </c>
       <c r="B27" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -4903,7 +5059,7 @@
         <v>124</v>
       </c>
       <c r="B31" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -4916,7 +5072,7 @@
         <v>126</v>
       </c>
       <c r="C33" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -4950,13 +5106,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>271</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
@@ -4989,7 +5145,7 @@
         <v>142</v>
       </c>
       <c r="B7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -4997,7 +5153,7 @@
         <v>135</v>
       </c>
       <c r="B8" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -5040,7 +5196,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -5051,13 +5207,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>271</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
@@ -5075,7 +5231,7 @@
         <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -5088,7 +5244,7 @@
         <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -5101,7 +5257,7 @@
         <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -5109,7 +5265,7 @@
         <v>95</v>
       </c>
       <c r="C9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -5122,7 +5278,7 @@
         <v>148</v>
       </c>
       <c r="B11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -5130,12 +5286,12 @@
         <v>144</v>
       </c>
       <c r="B12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -5148,7 +5304,7 @@
         <v>146</v>
       </c>
       <c r="B15" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -5156,7 +5312,7 @@
         <v>147</v>
       </c>
       <c r="B16" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -5169,7 +5325,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -5180,13 +5336,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>271</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
@@ -5214,7 +5370,7 @@
         <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -5227,7 +5383,7 @@
         <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -5240,7 +5396,7 @@
         <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -5248,7 +5404,7 @@
         <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -5266,7 +5422,7 @@
         <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -5284,7 +5440,7 @@
         <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -5292,7 +5448,7 @@
         <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -5317,10 +5473,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2796DC86-5C7A-4A1E-AE67-73CC08AECA93}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -5331,10 +5487,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
@@ -5342,28 +5498,35 @@
         <v>314</v>
       </c>
       <c r="B2" s="11">
-        <v>43559</v>
-      </c>
-      <c r="C2" t="s">
-        <v>316</v>
+        <v>43466</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B3" s="11">
+        <v>43559</v>
+      </c>
+      <c r="C3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="B3" s="11">
-        <v>43466</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
+      <c r="B4" s="5" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
+      <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
+      <c r="B6" s="5"/>
     </row>
     <row r="7" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
@@ -5376,17 +5539,15 @@
     </row>
     <row r="10" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
+      <c r="B10" s="9"/>
     </row>
     <row r="11" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
-      <c r="B11" s="9"/>
-    </row>
-    <row r="12" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5406,92 +5567,92 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>271</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B14" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -5515,13 +5676,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>271</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
@@ -5529,7 +5690,7 @@
         <v>152</v>
       </c>
       <c r="B2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -5537,7 +5698,7 @@
         <v>163</v>
       </c>
       <c r="B3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -5575,7 +5736,7 @@
         <v>167</v>
       </c>
       <c r="B10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -5588,7 +5749,7 @@
         <v>173</v>
       </c>
       <c r="B12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -5617,13 +5778,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>271</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
@@ -5631,7 +5792,7 @@
         <v>174</v>
       </c>
       <c r="B2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -5675,13 +5836,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>271</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
@@ -5689,7 +5850,7 @@
         <v>152</v>
       </c>
       <c r="B2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -5697,7 +5858,7 @@
         <v>173</v>
       </c>
       <c r="B3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -5771,13 +5932,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>271</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
@@ -5860,7 +6021,7 @@
         <v>197</v>
       </c>
       <c r="C17" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -5868,7 +6029,7 @@
         <v>205</v>
       </c>
       <c r="C18" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -5902,13 +6063,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>271</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
@@ -5921,7 +6082,7 @@
         <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -5970,18 +6131,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>271</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -5991,7 +6152,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -6004,7 +6165,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B12"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -6577,7 +6738,7 @@
         <v>222</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -7281,7 +7442,7 @@
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -7340,7 +7501,9 @@
         <v>132</v>
       </c>
       <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
+      <c r="C2" s="9">
+        <v>43678</v>
+      </c>
       <c r="D2" s="5"/>
       <c r="E2" s="10" t="s">
         <v>250</v>
@@ -7363,6 +7526,9 @@
     <row r="3" spans="1:14" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>133</v>
+      </c>
+      <c r="C3" s="9">
+        <v>43678</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="10"/>
@@ -7389,6 +7555,9 @@
       <c r="A4" s="2" t="s">
         <v>141</v>
       </c>
+      <c r="C4" s="9">
+        <v>43678</v>
+      </c>
       <c r="D4" s="5"/>
       <c r="E4" s="10"/>
       <c r="J4" s="5">
@@ -7409,10 +7578,11 @@
       <c r="A5" s="2" t="s">
         <v>134</v>
       </c>
+      <c r="C5" s="9">
+        <v>43678</v>
+      </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="10" t="s">
-        <v>251</v>
-      </c>
+      <c r="E5" s="10"/>
       <c r="F5" t="s">
         <v>58</v>
       </c>
@@ -7434,9 +7604,10 @@
       <c r="A6" s="2" t="s">
         <v>142</v>
       </c>
+      <c r="C6" s="9"/>
       <c r="D6" s="5"/>
       <c r="E6" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J6" s="5">
         <v>2</v>
@@ -7460,7 +7631,7 @@
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F7" t="s">
         <v>59</v>
@@ -7505,7 +7676,10 @@
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
+      </c>
+      <c r="F9" t="s">
+        <v>318</v>
       </c>
       <c r="J9" s="5">
         <v>2</v>
@@ -7528,8 +7702,8 @@
         <v>143</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" t="s">
-        <v>255</v>
+      <c r="E10" s="13" t="s">
+        <v>317</v>
       </c>
       <c r="F10" t="s">
         <v>56</v>
@@ -7742,6 +7916,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8067,8 +8242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA857DDD-2281-4A1A-9E85-5E0949545FD9}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -8125,10 +8300,12 @@
         <v>68</v>
       </c>
       <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
+      <c r="C2" s="9">
+        <v>43709</v>
+      </c>
       <c r="D2" s="5"/>
       <c r="E2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>67</v>
@@ -8153,9 +8330,12 @@
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="B3" s="9">
+        <v>43556</v>
+      </c>
       <c r="D3" s="5"/>
       <c r="E3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F3" t="s">
         <v>236</v>
@@ -8179,6 +8359,9 @@
     <row r="4" spans="1:13" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>70</v>
+      </c>
+      <c r="C4" s="9">
+        <v>43661</v>
       </c>
       <c r="D4" s="5"/>
       <c r="I4" s="5"/>
@@ -8215,7 +8398,7 @@
       </c>
       <c r="D7" s="5"/>
       <c r="E7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -8240,7 +8423,7 @@
       </c>
       <c r="D9" s="5"/>
       <c r="E9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -8252,12 +8435,15 @@
       <c r="A10" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="B10" s="9">
+        <v>43570</v>
+      </c>
       <c r="C10" s="9">
         <v>43709</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F10" t="s">
         <v>237</v>
@@ -8287,7 +8473,7 @@
       </c>
       <c r="D11" s="5"/>
       <c r="E11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -8327,7 +8513,7 @@
       </c>
       <c r="D14" s="5"/>
       <c r="E14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -8355,7 +8541,7 @@
       </c>
       <c r="D16" s="5"/>
       <c r="E16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -8677,7 +8863,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -8717,7 +8903,7 @@
       <c r="C2" s="9"/>
       <c r="D2" s="5"/>
       <c r="E2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F2" s="6"/>
     </row>
@@ -8727,7 +8913,7 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.2" x14ac:dyDescent="0.35">
@@ -8746,9 +8932,12 @@
       <c r="A6" s="2" t="s">
         <v>166</v>
       </c>
+      <c r="B6" s="9">
+        <v>43570</v>
+      </c>
       <c r="D6" s="5"/>
       <c r="E6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18.2" x14ac:dyDescent="0.35">
@@ -8757,7 +8946,7 @@
       </c>
       <c r="D7" s="5"/>
       <c r="E7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18.2" x14ac:dyDescent="0.35">
@@ -8880,12 +9069,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9047,15 +9233,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9BC95A6-9D68-4876-B344-5C0E9EA310F9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17C3FE88-FD63-422B-A211-481C065C3BEF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="a1bb4200-479c-4a05-afd7-28ce53bfa9b9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9079,17 +9276,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17C3FE88-FD63-422B-A211-481C065C3BEF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9BC95A6-9D68-4876-B344-5C0E9EA310F9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a1bb4200-479c-4a05-afd7-28ce53bfa9b9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Prognosis plot fixed for bug, and y_lim max is now better defined. Also added new box plot for measured catchmnets only.
</commit_message>
<xml_diff>
--- a/spring_flod_analysis.xlsx
+++ b/spring_flod_analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\personalfolders\MEHO\spring-flod-analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\energycorp\applications\OSL\jupyter_notebooks\personalfolders\MEHO\spring-flod-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A6829A-31F3-4CB9-9C90-2D54D62F44D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23719216-98B9-44EB-9AF1-06496C49A2CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18006" windowHeight="6699" tabRatio="860" activeTab="3" xr2:uid="{EB861DC1-2A69-4366-9E6B-67ADF5EDEFAB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18006" windowHeight="6699" tabRatio="860" activeTab="5" xr2:uid="{EB861DC1-2A69-4366-9E6B-67ADF5EDEFAB}"/>
   </bookViews>
   <sheets>
     <sheet name="user manual" sheetId="26" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="578">
   <si>
     <t>Område:</t>
   </si>
@@ -7718,7 +7718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EBF02F0-C4B4-4C24-81E7-9A77AA279C4F}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -9147,8 +9147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34551E16-052D-4A3D-BE1D-7C60BC1E7DC9}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -9222,9 +9222,7 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="5"/>
-      <c r="H2" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="H2" s="5"/>
       <c r="I2" s="6" t="s">
         <v>56</v>
       </c>
@@ -9250,9 +9248,7 @@
         <v>478</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="H3" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="H3" s="5"/>
       <c r="I3" s="6" t="s">
         <v>64</v>
       </c>
@@ -10354,12 +10350,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10521,15 +10514,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9BC95A6-9D68-4876-B344-5C0E9EA310F9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17C3FE88-FD63-422B-A211-481C065C3BEF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="a1bb4200-479c-4a05-afd7-28ce53bfa9b9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10553,17 +10557,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17C3FE88-FD63-422B-A211-481C065C3BEF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9BC95A6-9D68-4876-B344-5C0E9EA310F9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a1bb4200-479c-4a05-afd7-28ce53bfa9b9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added prognosis plot for Norge and Sweeden total.
</commit_message>
<xml_diff>
--- a/spring_flod_analysis.xlsx
+++ b/spring_flod_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\energycorp\applications\OSL\jupyter_notebooks\personalfolders\MEHO\spring-flod-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23719216-98B9-44EB-9AF1-06496C49A2CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF8A38F-0596-4425-9949-82BA62B9040F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18006" windowHeight="6699" tabRatio="860" activeTab="5" xr2:uid="{EB861DC1-2A69-4366-9E6B-67ADF5EDEFAB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="6705" tabRatio="860" activeTab="10" xr2:uid="{EB861DC1-2A69-4366-9E6B-67ADF5EDEFAB}"/>
   </bookViews>
   <sheets>
     <sheet name="user manual" sheetId="26" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="580">
   <si>
     <t>Område:</t>
   </si>
@@ -1789,6 +1789,12 @@
   </si>
   <si>
     <t>Snømåling:</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Kan oppdateres av og til med snømålinger fra Rana</t>
   </si>
 </sst>
 </file>
@@ -4752,7 +4758,7 @@
       <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4767,19 +4773,19 @@
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="177" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4808,7 +4814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>567</v>
       </c>
@@ -4826,7 +4832,7 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>576</v>
       </c>
@@ -4841,7 +4847,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>568</v>
       </c>
@@ -4851,7 +4857,7 @@
       <c r="E4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>569</v>
       </c>
@@ -4861,7 +4867,7 @@
       <c r="E5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>570</v>
       </c>
@@ -4871,116 +4877,116 @@
       <c r="E6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="E7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="E8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="E9" s="5"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="E10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="E11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="D12" s="9"/>
       <c r="E12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="E13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="E14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="E15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="E16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" s="5"/>
     </row>
   </sheetData>
@@ -4992,23 +4998,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C406E0-ACFC-4FD0-B0C6-C542CC72BC3D}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D37:D38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="192.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="192.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5037,7 +5043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>318</v>
       </c>
@@ -5051,12 +5057,10 @@
         <v>43692</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="H2" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="H2" s="5"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>319</v>
       </c>
@@ -5068,7 +5072,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>169</v>
       </c>
@@ -5079,7 +5083,7 @@
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>170</v>
       </c>
@@ -5090,7 +5094,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>320</v>
       </c>
@@ -5100,7 +5104,7 @@
       <c r="E6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>172</v>
       </c>
@@ -5111,7 +5115,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>173</v>
       </c>
@@ -5122,7 +5126,7 @@
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>174</v>
       </c>
@@ -5133,7 +5137,7 @@
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>321</v>
       </c>
@@ -5146,7 +5150,7 @@
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>322</v>
       </c>
@@ -5156,7 +5160,7 @@
       <c r="E11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>323</v>
       </c>
@@ -5170,7 +5174,7 @@
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>324</v>
       </c>
@@ -5186,7 +5190,7 @@
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>179</v>
       </c>
@@ -5195,11 +5199,9 @@
       <c r="G14" t="s">
         <v>309</v>
       </c>
-      <c r="H14" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>325</v>
       </c>
@@ -5212,7 +5214,7 @@
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>326</v>
       </c>
@@ -5225,7 +5227,7 @@
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>327</v>
       </c>
@@ -5235,7 +5237,7 @@
       <c r="E17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>328</v>
       </c>
@@ -5245,7 +5247,7 @@
       <c r="E18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>329</v>
       </c>
@@ -5255,7 +5257,7 @@
       <c r="E19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>184</v>
       </c>
@@ -5266,7 +5268,7 @@
       </c>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>185</v>
       </c>
@@ -5276,8 +5278,11 @@
         <v>311</v>
       </c>
       <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+      <c r="I21" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>330</v>
       </c>
@@ -5287,7 +5292,7 @@
       <c r="E22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>186</v>
       </c>
@@ -5298,7 +5303,7 @@
       </c>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>187</v>
       </c>
@@ -5309,7 +5314,7 @@
       </c>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>195</v>
       </c>
@@ -5320,7 +5325,7 @@
       </c>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>188</v>
       </c>
@@ -5329,11 +5334,9 @@
       <c r="G26" t="s">
         <v>315</v>
       </c>
-      <c r="H26" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>316</v>
       </c>
@@ -5343,7 +5346,7 @@
       <c r="E27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>332</v>
       </c>
@@ -5353,7 +5356,7 @@
       <c r="E28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>331</v>
       </c>
@@ -5363,7 +5366,7 @@
       <c r="E29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>192</v>
       </c>
@@ -5371,20 +5374,18 @@
       <c r="E30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>193</v>
       </c>
       <c r="B31" s="14"/>
       <c r="E31" s="5"/>
-      <c r="H31" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" s="5"/>
     </row>
   </sheetData>
@@ -5401,18 +5402,18 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="148.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="148.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5438,7 +5439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>233</v>
       </c>
@@ -5450,7 +5451,7 @@
       <c r="E2" s="5"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>225</v>
       </c>
@@ -5461,7 +5462,7 @@
       <c r="E3" s="5"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>226</v>
       </c>
@@ -5471,7 +5472,7 @@
       <c r="E4" s="5"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>227</v>
       </c>
@@ -5481,7 +5482,7 @@
       <c r="E5" s="5"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>228</v>
       </c>
@@ -5491,7 +5492,7 @@
       <c r="E6" s="5"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>229</v>
       </c>
@@ -5501,7 +5502,7 @@
       <c r="E7" s="5"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>230</v>
       </c>
@@ -5511,7 +5512,7 @@
       <c r="E8" s="5"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>231</v>
       </c>
@@ -5521,7 +5522,7 @@
       <c r="E9" s="5"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>232</v>
       </c>
@@ -5544,19 +5545,19 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="220.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="220.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5582,7 +5583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>234</v>
       </c>
@@ -5594,7 +5595,7 @@
       <c r="E2" s="5"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>225</v>
       </c>
@@ -5603,7 +5604,7 @@
       <c r="E3" s="5"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>226</v>
       </c>
@@ -5613,7 +5614,7 @@
       <c r="E4" s="5"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>227</v>
       </c>
@@ -5623,7 +5624,7 @@
       <c r="E5" s="5"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>228</v>
       </c>
@@ -5645,14 +5646,14 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.3" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>288</v>
       </c>
@@ -5661,7 +5662,7 @@
       </c>
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>284</v>
       </c>
@@ -5669,7 +5670,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>285</v>
       </c>
@@ -5677,7 +5678,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>287</v>
       </c>
@@ -5685,7 +5686,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>286</v>
       </c>
@@ -5693,7 +5694,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>281</v>
       </c>
@@ -5701,7 +5702,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>282</v>
       </c>
@@ -5709,7 +5710,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>279</v>
       </c>
@@ -5717,7 +5718,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>283</v>
       </c>
@@ -5738,13 +5739,13 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -5761,13 +5762,13 @@
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>83</v>
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -5775,7 +5776,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -5783,7 +5784,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -5792,25 +5793,25 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>86</v>
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>88</v>
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>98</v>
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>89</v>
       </c>
@@ -5819,19 +5820,19 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>90</v>
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>91</v>
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>92</v>
       </c>
@@ -5840,7 +5841,7 @@
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -5849,7 +5850,7 @@
       </c>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -5858,7 +5859,7 @@
       </c>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>96</v>
       </c>
@@ -5870,7 +5871,7 @@
       </c>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>111</v>
       </c>
@@ -5889,13 +5890,13 @@
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -5906,57 +5907,57 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>110</v>
       </c>
@@ -5964,42 +5965,42 @@
         <v>286</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>129</v>
       </c>
@@ -6007,12 +6008,12 @@
         <v>287</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>131</v>
       </c>
@@ -6020,12 +6021,12 @@
         <v>286</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>118</v>
       </c>
@@ -6033,7 +6034,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>259</v>
       </c>
@@ -6041,7 +6042,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>119</v>
       </c>
@@ -6049,7 +6050,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>120</v>
       </c>
@@ -6057,22 +6058,22 @@
         <v>287</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>124</v>
       </c>
@@ -6080,12 +6081,12 @@
         <v>286</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>126</v>
       </c>
@@ -6093,12 +6094,12 @@
         <v>282</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>133</v>
       </c>
@@ -6116,13 +6117,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -6133,32 +6134,32 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>142</v>
       </c>
@@ -6166,7 +6167,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>135</v>
       </c>
@@ -6174,32 +6175,32 @@
         <v>285</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>145</v>
       </c>
@@ -6217,13 +6218,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -6234,17 +6235,17 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -6252,12 +6253,12 @@
         <v>282</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -6265,12 +6266,12 @@
         <v>283</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>92</v>
       </c>
@@ -6278,7 +6279,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -6286,12 +6287,12 @@
         <v>279</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>148</v>
       </c>
@@ -6299,7 +6300,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>144</v>
       </c>
@@ -6307,17 +6308,17 @@
         <v>287</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>146</v>
       </c>
@@ -6325,7 +6326,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -6346,13 +6347,13 @@
       <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" customWidth="1"/>
-    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -6363,27 +6364,27 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -6391,12 +6392,12 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -6404,12 +6405,12 @@
         <v>279</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -6417,7 +6418,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -6425,17 +6426,17 @@
         <v>287</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -6443,17 +6444,17 @@
         <v>279</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -6461,7 +6462,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -6469,17 +6470,17 @@
         <v>287</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>150</v>
       </c>
@@ -6497,13 +6498,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>278</v>
       </c>
@@ -6511,7 +6512,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>339</v>
       </c>
@@ -6519,7 +6520,7 @@
         <v>43466</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>300</v>
       </c>
@@ -6530,32 +6531,32 @@
         <v>299</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="5"/>
     </row>
-    <row r="5" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="9"/>
     </row>
-    <row r="11" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
     </row>
   </sheetData>
@@ -6573,13 +6574,13 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -6590,27 +6591,27 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>265</v>
       </c>
@@ -6618,27 +6619,27 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>270</v>
       </c>
@@ -6646,17 +6647,17 @@
         <v>286</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>273</v>
       </c>
@@ -6664,7 +6665,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>274</v>
       </c>
@@ -6682,13 +6683,13 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -6699,7 +6700,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>149</v>
       </c>
@@ -6707,7 +6708,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>151</v>
       </c>
@@ -6715,37 +6716,37 @@
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -6753,12 +6754,12 @@
         <v>286</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>161</v>
       </c>
@@ -6766,7 +6767,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>156</v>
       </c>
@@ -6784,13 +6785,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -6801,7 +6802,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>162</v>
       </c>
@@ -6809,22 +6810,22 @@
         <v>285</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>165</v>
       </c>
@@ -6842,13 +6843,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -6859,7 +6860,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>149</v>
       </c>
@@ -6867,7 +6868,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>161</v>
       </c>
@@ -6875,52 +6876,52 @@
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>185</v>
       </c>
@@ -6938,13 +6939,13 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -6955,82 +6956,82 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>185</v>
       </c>
@@ -7038,7 +7039,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>192</v>
       </c>
@@ -7046,12 +7047,12 @@
         <v>281</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>187</v>
       </c>
@@ -7069,13 +7070,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -7086,12 +7087,12 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -7099,27 +7100,27 @@
         <v>281</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>181</v>
       </c>
@@ -7137,13 +7138,13 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -7154,17 +7155,17 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>276</v>
       </c>
@@ -7179,27 +7180,27 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="185" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7246,7 +7247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>372</v>
       </c>
@@ -7256,9 +7257,7 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="5"/>
-      <c r="H2" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="H2" s="5"/>
       <c r="I2" s="6" t="s">
         <v>12</v>
       </c>
@@ -7279,7 +7278,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>373</v>
       </c>
@@ -7308,7 +7307,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>374</v>
       </c>
@@ -7338,7 +7337,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>375</v>
       </c>
@@ -7365,7 +7364,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>376</v>
       </c>
@@ -7373,9 +7372,7 @@
         <v>351</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="H6" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="H6" s="5"/>
       <c r="I6" s="6"/>
       <c r="K6" s="2"/>
       <c r="L6" s="3"/>
@@ -7384,7 +7381,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>377</v>
       </c>
@@ -7392,9 +7389,7 @@
         <v>350</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="H7" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="H7" s="5"/>
       <c r="I7" s="6" t="s">
         <v>29</v>
       </c>
@@ -7411,7 +7406,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>378</v>
       </c>
@@ -7419,9 +7414,7 @@
         <v>349</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="H8" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="H8" s="5"/>
       <c r="I8" s="6"/>
       <c r="K8" s="2"/>
       <c r="L8" s="3"/>
@@ -7430,7 +7423,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>379</v>
       </c>
@@ -7447,7 +7440,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>380</v>
       </c>
@@ -7470,7 +7463,7 @@
       </c>
       <c r="P10" s="5"/>
     </row>
-    <row r="11" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>381</v>
       </c>
@@ -7481,9 +7474,7 @@
         <v>43508</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="H11" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="H11" s="5"/>
       <c r="I11" s="6" t="s">
         <v>27</v>
       </c>
@@ -7502,7 +7493,7 @@
       </c>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>382</v>
       </c>
@@ -7520,7 +7511,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>383</v>
       </c>
@@ -7552,7 +7543,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>384</v>
       </c>
@@ -7581,7 +7572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>385</v>
       </c>
@@ -7598,7 +7589,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>386</v>
       </c>
@@ -7627,7 +7618,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>387</v>
       </c>
@@ -7635,9 +7626,7 @@
         <v>347</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="H17" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="H17" s="5"/>
       <c r="I17" s="6" t="s">
         <v>26</v>
       </c>
@@ -7656,56 +7645,56 @@
       </c>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="E18" s="5"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="11:11" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="33" spans="11:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="11:11" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="34" spans="11:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K34" s="2"/>
     </row>
   </sheetData>
@@ -7718,29 +7707,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EBF02F0-C4B4-4C24-81E7-9A77AA279C4F}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="33.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="175.6640625" customWidth="1"/>
-    <col min="10" max="12" width="59.44140625" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="175.7109375" customWidth="1"/>
+    <col min="10" max="12" width="59.42578125" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7787,7 +7776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>388</v>
       </c>
@@ -7801,9 +7790,7 @@
         <v>43631</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="H2" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="H2" s="5"/>
       <c r="I2" s="6" t="s">
         <v>33</v>
       </c>
@@ -7826,7 +7813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>389</v>
       </c>
@@ -7858,7 +7845,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>390</v>
       </c>
@@ -7871,7 +7858,9 @@
       <c r="F4" t="s">
         <v>209</v>
       </c>
-      <c r="H4" s="5"/>
+      <c r="H4" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I4" s="6" t="s">
         <v>290</v>
       </c>
@@ -7894,7 +7883,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>391</v>
       </c>
@@ -7917,7 +7906,7 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>392</v>
       </c>
@@ -7925,9 +7914,7 @@
         <v>423</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="H6" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="H6" s="5"/>
       <c r="I6" s="6" t="s">
         <v>36</v>
       </c>
@@ -7944,7 +7931,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>393</v>
       </c>
@@ -7952,9 +7939,7 @@
         <v>424</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="H7" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="H7" s="5"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
@@ -7969,7 +7954,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>394</v>
       </c>
@@ -7977,9 +7962,7 @@
         <v>425</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="H8" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="H8" s="5"/>
       <c r="I8" s="6" t="s">
         <v>37</v>
       </c>
@@ -8000,7 +7983,7 @@
       </c>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>395</v>
       </c>
@@ -8032,7 +8015,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>396</v>
       </c>
@@ -8046,7 +8029,9 @@
       <c r="F10" t="s">
         <v>210</v>
       </c>
-      <c r="H10" s="5"/>
+      <c r="H10" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I10" s="6" t="s">
         <v>38</v>
       </c>
@@ -8069,7 +8054,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>397</v>
       </c>
@@ -8094,7 +8079,7 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>109</v>
       </c>
@@ -8124,7 +8109,7 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>398</v>
       </c>
@@ -8155,7 +8140,7 @@
       </c>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>399</v>
       </c>
@@ -8186,7 +8171,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>400</v>
       </c>
@@ -8194,7 +8179,9 @@
         <v>431</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="H15" s="5"/>
+      <c r="H15" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I15" s="6" t="s">
         <v>44</v>
       </c>
@@ -8217,7 +8204,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>401</v>
       </c>
@@ -8225,7 +8212,9 @@
         <v>432</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="H16" s="5"/>
+      <c r="H16" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
@@ -8244,7 +8233,7 @@
       </c>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>402</v>
       </c>
@@ -8276,7 +8265,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>403</v>
       </c>
@@ -8290,7 +8279,9 @@
       <c r="G18" t="s">
         <v>451</v>
       </c>
-      <c r="H18" s="5"/>
+      <c r="H18" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I18" s="6" t="s">
         <v>47</v>
       </c>
@@ -8307,7 +8298,7 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>404</v>
       </c>
@@ -8318,14 +8309,16 @@
       <c r="F19" t="s">
         <v>213</v>
       </c>
-      <c r="H19" s="5"/>
+      <c r="H19" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>405</v>
       </c>
@@ -8340,7 +8333,7 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>406</v>
       </c>
@@ -8351,7 +8344,9 @@
       <c r="F21" t="s">
         <v>214</v>
       </c>
-      <c r="H21" s="5"/>
+      <c r="H21" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I21" t="s">
         <v>48</v>
       </c>
@@ -8369,7 +8364,7 @@
       </c>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>407</v>
       </c>
@@ -8377,7 +8372,9 @@
         <v>438</v>
       </c>
       <c r="E22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="H22" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I22" t="s">
         <v>49</v>
       </c>
@@ -8391,7 +8388,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>408</v>
       </c>
@@ -8402,7 +8399,9 @@
       <c r="F23" t="s">
         <v>215</v>
       </c>
-      <c r="H23" s="5"/>
+      <c r="H23" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I23" t="s">
         <v>50</v>
       </c>
@@ -8422,7 +8421,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>409</v>
       </c>
@@ -8433,7 +8432,9 @@
       <c r="F24" t="s">
         <v>216</v>
       </c>
-      <c r="H24" s="5"/>
+      <c r="H24" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="M24" s="5">
         <v>2</v>
       </c>
@@ -8448,7 +8449,7 @@
       </c>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>410</v>
       </c>
@@ -8459,7 +8460,9 @@
       <c r="F25" t="s">
         <v>217</v>
       </c>
-      <c r="H25" s="5"/>
+      <c r="H25" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I25" t="s">
         <v>51</v>
       </c>
@@ -8479,7 +8482,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>411</v>
       </c>
@@ -8490,7 +8493,9 @@
       <c r="F26" t="s">
         <v>218</v>
       </c>
-      <c r="H26" s="5"/>
+      <c r="H26" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I26" t="s">
         <v>52</v>
       </c>
@@ -8510,7 +8515,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>120</v>
       </c>
@@ -8522,7 +8527,7 @@
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>412</v>
       </c>
@@ -8537,7 +8542,7 @@
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
     </row>
-    <row r="29" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>413</v>
       </c>
@@ -8548,7 +8553,9 @@
       <c r="F29" t="s">
         <v>219</v>
       </c>
-      <c r="H29" s="5"/>
+      <c r="H29" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="M29" s="5">
         <v>1</v>
       </c>
@@ -8563,7 +8570,7 @@
       </c>
       <c r="Q29" s="5"/>
     </row>
-    <row r="30" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>414</v>
       </c>
@@ -8591,7 +8598,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>415</v>
       </c>
@@ -8601,7 +8608,9 @@
       <c r="E31" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="H31" s="5"/>
+      <c r="H31" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I31" t="s">
         <v>54</v>
       </c>
@@ -8613,7 +8622,7 @@
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
     </row>
-    <row r="32" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>416</v>
       </c>
@@ -8621,7 +8630,9 @@
         <v>447</v>
       </c>
       <c r="E32" s="5"/>
-      <c r="H32" s="5"/>
+      <c r="H32" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I32" t="s">
         <v>55</v>
       </c>
@@ -8639,7 +8650,7 @@
       </c>
       <c r="Q32" s="5"/>
     </row>
-    <row r="33" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>417</v>
       </c>
@@ -8650,7 +8661,9 @@
       <c r="F33" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="H33" s="5"/>
+      <c r="H33" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I33" s="8" t="s">
         <v>197</v>
       </c>
@@ -8673,7 +8686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>418</v>
       </c>
@@ -8686,7 +8699,9 @@
       <c r="G34" t="s">
         <v>452</v>
       </c>
-      <c r="H34" s="5"/>
+      <c r="H34" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="M34" s="5">
         <v>2</v>
       </c>
@@ -8712,28 +8727,28 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="179.44140625" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="179.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8778,7 +8793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>465</v>
       </c>
@@ -8811,7 +8826,7 @@
       </c>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>466</v>
       </c>
@@ -8823,9 +8838,7 @@
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="10"/>
-      <c r="H3" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="H3" s="5"/>
       <c r="I3" t="s">
         <v>56</v>
       </c>
@@ -8845,7 +8858,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>467</v>
       </c>
@@ -8872,7 +8885,7 @@
       </c>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>468</v>
       </c>
@@ -8884,7 +8897,9 @@
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="10"/>
-      <c r="H5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I5" t="s">
         <v>58</v>
       </c>
@@ -8902,7 +8917,7 @@
       </c>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>469</v>
       </c>
@@ -8933,7 +8948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>470</v>
       </c>
@@ -8964,7 +8979,7 @@
       </c>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>471</v>
       </c>
@@ -8973,9 +8988,7 @@
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="10"/>
-      <c r="H8" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="H8" s="5"/>
       <c r="M8" s="5">
         <v>1</v>
       </c>
@@ -8990,7 +9003,7 @@
       </c>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>472</v>
       </c>
@@ -9001,7 +9014,9 @@
       <c r="F9" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="H9" s="5"/>
+      <c r="H9" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I9" t="s">
         <v>302</v>
       </c>
@@ -9021,7 +9036,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>473</v>
       </c>
@@ -9032,7 +9047,9 @@
       <c r="F10" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="H10" s="5"/>
+      <c r="H10" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I10" t="s">
         <v>56</v>
       </c>
@@ -9051,7 +9068,7 @@
       </c>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>474</v>
       </c>
@@ -9060,9 +9077,7 @@
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="10"/>
-      <c r="H11" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="H11" s="5"/>
       <c r="I11" t="s">
         <v>61</v>
       </c>
@@ -9080,7 +9095,7 @@
       </c>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>475</v>
       </c>
@@ -9111,7 +9126,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>476</v>
       </c>
@@ -9147,28 +9162,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34551E16-052D-4A3D-BE1D-7C60BC1E7DC9}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="179.5546875" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="179.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9212,7 +9227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>481</v>
       </c>
@@ -9240,7 +9255,7 @@
       </c>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="1:14" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>450</v>
       </c>
@@ -9268,7 +9283,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>482</v>
       </c>
@@ -9279,7 +9294,9 @@
       <c r="F4" t="s">
         <v>199</v>
       </c>
-      <c r="H4" s="5"/>
+      <c r="H4" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I4" s="6" t="s">
         <v>65</v>
       </c>
@@ -9297,7 +9314,7 @@
       </c>
       <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="1:14" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>483</v>
       </c>
@@ -9308,7 +9325,9 @@
       <c r="F5" t="s">
         <v>200</v>
       </c>
-      <c r="H5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I5" s="6"/>
       <c r="J5" s="5">
         <v>3</v>
@@ -9324,12 +9343,14 @@
       </c>
       <c r="N5" s="5"/>
     </row>
-    <row r="6" spans="1:14" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>148</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I6" s="6"/>
       <c r="J6" s="5">
         <v>3</v>
@@ -9345,10 +9366,10 @@
       </c>
       <c r="N6" s="5"/>
     </row>
-    <row r="7" spans="1:14" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:14" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
     </row>
   </sheetData>
@@ -9361,27 +9382,27 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="201" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9425,7 +9446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>499</v>
       </c>
@@ -9462,7 +9483,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>500</v>
       </c>
@@ -9498,7 +9519,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>501</v>
       </c>
@@ -9516,7 +9537,7 @@
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>502</v>
       </c>
@@ -9531,7 +9552,7 @@
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>503</v>
       </c>
@@ -9546,7 +9567,7 @@
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>504</v>
       </c>
@@ -9557,14 +9578,16 @@
       <c r="F7" t="s">
         <v>243</v>
       </c>
-      <c r="H7" s="5"/>
+      <c r="H7" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>505</v>
       </c>
@@ -9572,14 +9595,16 @@
         <v>490</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="H8" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>506</v>
       </c>
@@ -9590,14 +9615,16 @@
       <c r="F9" t="s">
         <v>244</v>
       </c>
-      <c r="H9" s="5"/>
+      <c r="H9" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>507</v>
       </c>
@@ -9615,7 +9642,7 @@
         <v>245</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>206</v>
+        <v>578</v>
       </c>
       <c r="I10" t="s">
         <v>224</v>
@@ -9636,7 +9663,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>508</v>
       </c>
@@ -9650,14 +9677,16 @@
       <c r="F11" t="s">
         <v>246</v>
       </c>
-      <c r="H11" s="5"/>
+      <c r="H11" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>509</v>
       </c>
@@ -9673,7 +9702,7 @@
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>510</v>
       </c>
@@ -9691,7 +9720,7 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>511</v>
       </c>
@@ -9702,14 +9731,16 @@
       <c r="F14" t="s">
         <v>247</v>
       </c>
-      <c r="H14" s="5"/>
+      <c r="H14" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>512</v>
       </c>
@@ -9726,7 +9757,7 @@
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>513</v>
       </c>
@@ -9740,91 +9771,93 @@
       <c r="F16" t="s">
         <v>248</v>
       </c>
-      <c r="H16" s="5"/>
+      <c r="H16" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
     </row>
   </sheetData>
@@ -9838,23 +9871,23 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.109375" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9883,7 +9916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>514</v>
       </c>
@@ -9893,12 +9926,10 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="5"/>
-      <c r="H2" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="H2" s="5"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>515</v>
       </c>
@@ -9910,7 +9941,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>516</v>
       </c>
@@ -9920,7 +9951,7 @@
       <c r="E4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>517</v>
       </c>
@@ -9930,7 +9961,7 @@
       <c r="E5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>518</v>
       </c>
@@ -9941,12 +9972,14 @@
       <c r="F6" t="s">
         <v>196</v>
       </c>
-      <c r="H6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="I6" s="8" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>519</v>
       </c>
@@ -9956,7 +9989,7 @@
       <c r="E7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>520</v>
       </c>
@@ -9966,7 +9999,7 @@
       <c r="E8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>521</v>
       </c>
@@ -9977,9 +10010,11 @@
       <c r="G9" t="s">
         <v>542</v>
       </c>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
+      <c r="H9" s="5" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>522</v>
       </c>
@@ -9995,7 +10030,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>523</v>
       </c>
@@ -10007,9 +10042,11 @@
       <c r="F11" t="s">
         <v>203</v>
       </c>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
+      <c r="H11" s="5" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>544</v>
       </c>
@@ -10024,9 +10061,11 @@
       <c r="G12" t="s">
         <v>524</v>
       </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
+      <c r="H12" s="5" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>525</v>
       </c>
@@ -10037,7 +10076,7 @@
       <c r="E13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>526</v>
       </c>
@@ -10048,10 +10087,12 @@
       <c r="F14" t="s">
         <v>201</v>
       </c>
-      <c r="H14" s="5"/>
+      <c r="H14" s="5" t="s">
+        <v>578</v>
+      </c>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>527</v>
       </c>
@@ -10062,80 +10103,78 @@
         <v>43507</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="H15" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="E16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:1" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
     </row>
   </sheetData>
@@ -10148,23 +10187,23 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="179.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="179.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10193,7 +10232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>556</v>
       </c>
@@ -10211,7 +10250,7 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>557</v>
       </c>
@@ -10226,7 +10265,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>558</v>
       </c>
@@ -10234,9 +10273,11 @@
         <v>547</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+      <c r="H4" s="5" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>559</v>
       </c>
@@ -10246,7 +10287,7 @@
       <c r="E5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>560</v>
       </c>
@@ -10260,9 +10301,11 @@
       <c r="F6" t="s">
         <v>251</v>
       </c>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+      <c r="H6" s="5" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>561</v>
       </c>
@@ -10273,9 +10316,11 @@
       <c r="F7" t="s">
         <v>252</v>
       </c>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+      <c r="H7" s="5" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>566</v>
       </c>
@@ -10283,9 +10328,11 @@
         <v>551</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+      <c r="H8" s="5" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>562</v>
       </c>
@@ -10295,7 +10342,7 @@
       <c r="E9" s="5"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>563</v>
       </c>
@@ -10303,11 +10350,9 @@
         <v>553</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="H10" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>564</v>
       </c>
@@ -10317,7 +10362,7 @@
       <c r="E11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>565</v>
       </c>
@@ -10331,16 +10376,16 @@
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H16" s="5"/>
     </row>
   </sheetData>
@@ -10350,9 +10395,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10514,26 +10562,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17C3FE88-FD63-422B-A211-481C065C3BEF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9BC95A6-9D68-4876-B344-5C0E9EA310F9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a1bb4200-479c-4a05-afd7-28ce53bfa9b9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10557,9 +10594,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9BC95A6-9D68-4876-B344-5C0E9EA310F9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17C3FE88-FD63-422B-A211-481C065C3BEF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="a1bb4200-479c-4a05-afd7-28ce53bfa9b9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added pretty print of pie plot numbers.
</commit_message>
<xml_diff>
--- a/spring_flod_analysis.xlsx
+++ b/spring_flod_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\energycorp\applications\OSL\jupyter_notebooks\personalfolders\MEHO\spring-flod-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF8A38F-0596-4425-9949-82BA62B9040F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76253D53-0A5C-4CDB-9FB8-9F5D5F2B89FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="6705" tabRatio="860" activeTab="10" xr2:uid="{EB861DC1-2A69-4366-9E6B-67ADF5EDEFAB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18006" windowHeight="6699" tabRatio="860" activeTab="10" xr2:uid="{EB861DC1-2A69-4366-9E6B-67ADF5EDEFAB}"/>
   </bookViews>
   <sheets>
     <sheet name="user manual" sheetId="26" r:id="rId1"/>
@@ -4758,7 +4758,7 @@
       <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4770,22 +4770,22 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="177" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>567</v>
       </c>
@@ -4832,7 +4832,7 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>576</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>568</v>
       </c>
@@ -4857,7 +4857,7 @@
       <c r="E4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>569</v>
       </c>
@@ -4867,7 +4867,7 @@
       <c r="E5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>570</v>
       </c>
@@ -4877,116 +4877,116 @@
       <c r="E6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="E7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="E8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="E9" s="5"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="E10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="E11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="D12" s="9"/>
       <c r="E12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="E13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="E14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="E15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="E16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E33" s="5"/>
     </row>
   </sheetData>
@@ -4998,23 +4998,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C406E0-ACFC-4FD0-B0C6-C542CC72BC3D}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="192.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="192.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>318</v>
       </c>
@@ -5060,7 +5060,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>319</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>169</v>
       </c>
@@ -5083,7 +5083,7 @@
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>170</v>
       </c>
@@ -5094,7 +5094,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>320</v>
       </c>
@@ -5104,7 +5104,7 @@
       <c r="E6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>172</v>
       </c>
@@ -5115,7 +5115,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>173</v>
       </c>
@@ -5126,7 +5126,7 @@
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>174</v>
       </c>
@@ -5137,7 +5137,7 @@
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>321</v>
       </c>
@@ -5150,7 +5150,7 @@
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>322</v>
       </c>
@@ -5160,7 +5160,7 @@
       <c r="E11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>323</v>
       </c>
@@ -5174,7 +5174,7 @@
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>324</v>
       </c>
@@ -5190,7 +5190,7 @@
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>179</v>
       </c>
@@ -5201,7 +5201,7 @@
       </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>325</v>
       </c>
@@ -5214,7 +5214,7 @@
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>326</v>
       </c>
@@ -5227,7 +5227,7 @@
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>327</v>
       </c>
@@ -5237,7 +5237,7 @@
       <c r="E17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>328</v>
       </c>
@@ -5247,7 +5247,7 @@
       <c r="E18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>329</v>
       </c>
@@ -5257,7 +5257,7 @@
       <c r="E19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>184</v>
       </c>
@@ -5268,7 +5268,7 @@
       </c>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>185</v>
       </c>
@@ -5282,7 +5282,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>330</v>
       </c>
@@ -5292,7 +5292,7 @@
       <c r="E22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>186</v>
       </c>
@@ -5303,7 +5303,7 @@
       </c>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>187</v>
       </c>
@@ -5314,7 +5314,7 @@
       </c>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>195</v>
       </c>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>188</v>
       </c>
@@ -5336,7 +5336,7 @@
       </c>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>316</v>
       </c>
@@ -5346,7 +5346,7 @@
       <c r="E27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>332</v>
       </c>
@@ -5356,7 +5356,7 @@
       <c r="E28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>331</v>
       </c>
@@ -5366,7 +5366,7 @@
       <c r="E29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>192</v>
       </c>
@@ -5374,7 +5374,7 @@
       <c r="E30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>193</v>
       </c>
@@ -5382,10 +5382,10 @@
       <c r="E31" s="5"/>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E33" s="5"/>
     </row>
   </sheetData>
@@ -5402,18 +5402,18 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="148.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="148.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5439,7 +5439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>233</v>
       </c>
@@ -5451,7 +5451,7 @@
       <c r="E2" s="5"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>225</v>
       </c>
@@ -5462,7 +5462,7 @@
       <c r="E3" s="5"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>226</v>
       </c>
@@ -5472,7 +5472,7 @@
       <c r="E4" s="5"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>227</v>
       </c>
@@ -5482,7 +5482,7 @@
       <c r="E5" s="5"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>228</v>
       </c>
@@ -5492,7 +5492,7 @@
       <c r="E6" s="5"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>229</v>
       </c>
@@ -5502,7 +5502,7 @@
       <c r="E7" s="5"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>230</v>
       </c>
@@ -5512,7 +5512,7 @@
       <c r="E8" s="5"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>231</v>
       </c>
@@ -5522,7 +5522,7 @@
       <c r="E9" s="5"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>232</v>
       </c>
@@ -5545,19 +5545,19 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="220.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="220.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>234</v>
       </c>
@@ -5595,7 +5595,7 @@
       <c r="E2" s="5"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>225</v>
       </c>
@@ -5604,7 +5604,7 @@
       <c r="E3" s="5"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>226</v>
       </c>
@@ -5614,7 +5614,7 @@
       <c r="E4" s="5"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>227</v>
       </c>
@@ -5624,7 +5624,7 @@
       <c r="E5" s="5"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>228</v>
       </c>
@@ -5646,14 +5646,14 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16.3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>288</v>
       </c>
@@ -5662,7 +5662,7 @@
       </c>
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>284</v>
       </c>
@@ -5670,7 +5670,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>285</v>
       </c>
@@ -5678,7 +5678,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>287</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>286</v>
       </c>
@@ -5694,7 +5694,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>281</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>282</v>
       </c>
@@ -5710,7 +5710,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>279</v>
       </c>
@@ -5718,7 +5718,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>283</v>
       </c>
@@ -5739,13 +5739,13 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -5762,13 +5762,13 @@
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>83</v>
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -5776,7 +5776,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -5793,25 +5793,25 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>86</v>
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>88</v>
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>98</v>
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>89</v>
       </c>
@@ -5820,19 +5820,19 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>90</v>
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>91</v>
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>92</v>
       </c>
@@ -5841,7 +5841,7 @@
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -5850,7 +5850,7 @@
       </c>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -5859,7 +5859,7 @@
       </c>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>96</v>
       </c>
@@ -5871,7 +5871,7 @@
       </c>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>111</v>
       </c>
@@ -5890,13 +5890,13 @@
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -5907,57 +5907,57 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>110</v>
       </c>
@@ -5965,42 +5965,42 @@
         <v>286</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>129</v>
       </c>
@@ -6008,12 +6008,12 @@
         <v>287</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>131</v>
       </c>
@@ -6021,12 +6021,12 @@
         <v>286</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>118</v>
       </c>
@@ -6034,7 +6034,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>259</v>
       </c>
@@ -6042,7 +6042,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>119</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>120</v>
       </c>
@@ -6058,22 +6058,22 @@
         <v>287</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>124</v>
       </c>
@@ -6081,12 +6081,12 @@
         <v>286</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>126</v>
       </c>
@@ -6094,12 +6094,12 @@
         <v>282</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>133</v>
       </c>
@@ -6117,13 +6117,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -6134,32 +6134,32 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>142</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>135</v>
       </c>
@@ -6175,32 +6175,32 @@
         <v>285</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>145</v>
       </c>
@@ -6218,13 +6218,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -6235,17 +6235,17 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -6253,12 +6253,12 @@
         <v>282</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -6266,12 +6266,12 @@
         <v>283</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>92</v>
       </c>
@@ -6279,7 +6279,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -6287,12 +6287,12 @@
         <v>279</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>148</v>
       </c>
@@ -6300,7 +6300,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>144</v>
       </c>
@@ -6308,17 +6308,17 @@
         <v>287</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>146</v>
       </c>
@@ -6326,7 +6326,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -6347,13 +6347,13 @@
       <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -6364,27 +6364,27 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -6392,12 +6392,12 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -6405,12 +6405,12 @@
         <v>279</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -6418,7 +6418,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -6426,17 +6426,17 @@
         <v>287</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -6444,17 +6444,17 @@
         <v>279</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -6462,7 +6462,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -6470,17 +6470,17 @@
         <v>287</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>150</v>
       </c>
@@ -6498,13 +6498,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>278</v>
       </c>
@@ -6512,7 +6512,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>339</v>
       </c>
@@ -6520,7 +6520,7 @@
         <v>43466</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>300</v>
       </c>
@@ -6531,32 +6531,32 @@
         <v>299</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="5"/>
     </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="9"/>
     </row>
-    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
     </row>
   </sheetData>
@@ -6574,13 +6574,13 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -6591,27 +6591,27 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>265</v>
       </c>
@@ -6619,27 +6619,27 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>270</v>
       </c>
@@ -6647,17 +6647,17 @@
         <v>286</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>273</v>
       </c>
@@ -6665,7 +6665,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>274</v>
       </c>
@@ -6683,13 +6683,13 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -6700,7 +6700,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>149</v>
       </c>
@@ -6708,7 +6708,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>151</v>
       </c>
@@ -6716,37 +6716,37 @@
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -6754,12 +6754,12 @@
         <v>286</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>161</v>
       </c>
@@ -6767,7 +6767,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>156</v>
       </c>
@@ -6785,13 +6785,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -6802,7 +6802,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>162</v>
       </c>
@@ -6810,22 +6810,22 @@
         <v>285</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>165</v>
       </c>
@@ -6843,13 +6843,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -6860,7 +6860,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>149</v>
       </c>
@@ -6868,7 +6868,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>161</v>
       </c>
@@ -6876,52 +6876,52 @@
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>185</v>
       </c>
@@ -6939,13 +6939,13 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -6956,82 +6956,82 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>185</v>
       </c>
@@ -7039,7 +7039,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>192</v>
       </c>
@@ -7047,12 +7047,12 @@
         <v>281</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>187</v>
       </c>
@@ -7070,13 +7070,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -7087,12 +7087,12 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -7100,27 +7100,27 @@
         <v>281</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>181</v>
       </c>
@@ -7138,13 +7138,13 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -7155,17 +7155,17 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>276</v>
       </c>
@@ -7183,24 +7183,24 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="185" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7247,7 +7247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>372</v>
       </c>
@@ -7278,7 +7278,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>373</v>
       </c>
@@ -7307,7 +7307,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>374</v>
       </c>
@@ -7337,7 +7337,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>375</v>
       </c>
@@ -7364,7 +7364,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>376</v>
       </c>
@@ -7381,7 +7381,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>377</v>
       </c>
@@ -7406,7 +7406,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>378</v>
       </c>
@@ -7423,7 +7423,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>379</v>
       </c>
@@ -7440,7 +7440,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>380</v>
       </c>
@@ -7463,7 +7463,7 @@
       </c>
       <c r="P10" s="5"/>
     </row>
-    <row r="11" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>381</v>
       </c>
@@ -7493,7 +7493,7 @@
       </c>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>382</v>
       </c>
@@ -7511,7 +7511,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>383</v>
       </c>
@@ -7543,7 +7543,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>384</v>
       </c>
@@ -7572,7 +7572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>385</v>
       </c>
@@ -7589,7 +7589,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>386</v>
       </c>
@@ -7618,7 +7618,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>387</v>
       </c>
@@ -7645,56 +7645,56 @@
       </c>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="E18" s="5"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="11:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="11:11" ht="18.2" x14ac:dyDescent="0.35">
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="11:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="11:11" ht="18.2" x14ac:dyDescent="0.35">
       <c r="K34" s="2"/>
     </row>
   </sheetData>
@@ -7707,29 +7707,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EBF02F0-C4B4-4C24-81E7-9A77AA279C4F}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="175.7109375" customWidth="1"/>
-    <col min="10" max="12" width="59.42578125" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="33.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="175.6640625" customWidth="1"/>
+    <col min="10" max="12" width="59.44140625" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7776,7 +7776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>388</v>
       </c>
@@ -7813,7 +7813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>389</v>
       </c>
@@ -7845,7 +7845,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>390</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>391</v>
       </c>
@@ -7906,7 +7906,7 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>392</v>
       </c>
@@ -7931,7 +7931,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>393</v>
       </c>
@@ -7954,7 +7954,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>394</v>
       </c>
@@ -7983,7 +7983,7 @@
       </c>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>395</v>
       </c>
@@ -8015,7 +8015,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>396</v>
       </c>
@@ -8054,7 +8054,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>397</v>
       </c>
@@ -8079,7 +8079,7 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>109</v>
       </c>
@@ -8109,7 +8109,7 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>398</v>
       </c>
@@ -8140,7 +8140,7 @@
       </c>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>399</v>
       </c>
@@ -8171,7 +8171,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>400</v>
       </c>
@@ -8204,7 +8204,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>401</v>
       </c>
@@ -8233,7 +8233,7 @@
       </c>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>402</v>
       </c>
@@ -8265,7 +8265,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>403</v>
       </c>
@@ -8298,7 +8298,7 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>404</v>
       </c>
@@ -8318,7 +8318,7 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>405</v>
       </c>
@@ -8333,7 +8333,7 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>406</v>
       </c>
@@ -8364,7 +8364,7 @@
       </c>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>407</v>
       </c>
@@ -8388,7 +8388,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>408</v>
       </c>
@@ -8421,7 +8421,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>409</v>
       </c>
@@ -8449,7 +8449,7 @@
       </c>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>410</v>
       </c>
@@ -8482,7 +8482,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>411</v>
       </c>
@@ -8515,7 +8515,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>120</v>
       </c>
@@ -8527,7 +8527,7 @@
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>412</v>
       </c>
@@ -8542,7 +8542,7 @@
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
     </row>
-    <row r="29" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>413</v>
       </c>
@@ -8554,7 +8554,7 @@
         <v>219</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="M29" s="5">
         <v>1</v>
@@ -8570,7 +8570,7 @@
       </c>
       <c r="Q29" s="5"/>
     </row>
-    <row r="30" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>414</v>
       </c>
@@ -8598,7 +8598,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>415</v>
       </c>
@@ -8609,7 +8609,7 @@
         <v>206</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="I31" t="s">
         <v>54</v>
@@ -8622,7 +8622,7 @@
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
     </row>
-    <row r="32" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>416</v>
       </c>
@@ -8631,7 +8631,7 @@
       </c>
       <c r="E32" s="5"/>
       <c r="H32" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="I32" t="s">
         <v>55</v>
@@ -8650,7 +8650,7 @@
       </c>
       <c r="Q32" s="5"/>
     </row>
-    <row r="33" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>417</v>
       </c>
@@ -8662,7 +8662,7 @@
         <v>198</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="I33" s="8" t="s">
         <v>197</v>
@@ -8686,7 +8686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>418</v>
       </c>
@@ -8700,7 +8700,7 @@
         <v>452</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="M34" s="5">
         <v>2</v>
@@ -8727,28 +8727,28 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="179.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="179.44140625" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8793,7 +8793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>465</v>
       </c>
@@ -8826,7 +8826,7 @@
       </c>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>466</v>
       </c>
@@ -8858,7 +8858,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>467</v>
       </c>
@@ -8885,7 +8885,7 @@
       </c>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>468</v>
       </c>
@@ -8898,7 +8898,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="10"/>
       <c r="H5" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="I5" t="s">
         <v>58</v>
@@ -8917,7 +8917,7 @@
       </c>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>469</v>
       </c>
@@ -8948,7 +8948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>470</v>
       </c>
@@ -8979,7 +8979,7 @@
       </c>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>471</v>
       </c>
@@ -9003,7 +9003,7 @@
       </c>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>472</v>
       </c>
@@ -9015,7 +9015,7 @@
         <v>240</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="I9" t="s">
         <v>302</v>
@@ -9036,7 +9036,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>473</v>
       </c>
@@ -9048,7 +9048,7 @@
         <v>301</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="I10" t="s">
         <v>56</v>
@@ -9068,7 +9068,7 @@
       </c>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>474</v>
       </c>
@@ -9095,7 +9095,7 @@
       </c>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>475</v>
       </c>
@@ -9126,7 +9126,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>476</v>
       </c>
@@ -9163,27 +9163,27 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="179.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="179.5546875" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9227,7 +9227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>481</v>
       </c>
@@ -9255,7 +9255,7 @@
       </c>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>450</v>
       </c>
@@ -9283,7 +9283,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>482</v>
       </c>
@@ -9295,7 +9295,7 @@
         <v>199</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>65</v>
@@ -9314,7 +9314,7 @@
       </c>
       <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>483</v>
       </c>
@@ -9326,7 +9326,7 @@
         <v>200</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="5">
@@ -9343,13 +9343,13 @@
       </c>
       <c r="N5" s="5"/>
     </row>
-    <row r="6" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>148</v>
       </c>
       <c r="E6" s="5"/>
       <c r="H6" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="5">
@@ -9366,10 +9366,10 @@
       </c>
       <c r="N6" s="5"/>
     </row>
-    <row r="7" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
     </row>
   </sheetData>
@@ -9382,27 +9382,27 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="201" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9446,7 +9446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>499</v>
       </c>
@@ -9483,7 +9483,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>500</v>
       </c>
@@ -9519,7 +9519,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>501</v>
       </c>
@@ -9537,7 +9537,7 @@
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>502</v>
       </c>
@@ -9552,7 +9552,7 @@
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>503</v>
       </c>
@@ -9567,7 +9567,7 @@
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>504</v>
       </c>
@@ -9579,7 +9579,7 @@
         <v>243</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
@@ -9587,7 +9587,7 @@
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>505</v>
       </c>
@@ -9596,7 +9596,7 @@
       </c>
       <c r="E8" s="5"/>
       <c r="H8" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
@@ -9604,7 +9604,7 @@
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>506</v>
       </c>
@@ -9616,7 +9616,7 @@
         <v>244</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
@@ -9624,7 +9624,7 @@
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>507</v>
       </c>
@@ -9642,7 +9642,7 @@
         <v>245</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="I10" t="s">
         <v>224</v>
@@ -9663,7 +9663,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>508</v>
       </c>
@@ -9678,7 +9678,7 @@
         <v>246</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -9686,7 +9686,7 @@
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>509</v>
       </c>
@@ -9702,7 +9702,7 @@
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>510</v>
       </c>
@@ -9720,7 +9720,7 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>511</v>
       </c>
@@ -9732,7 +9732,7 @@
         <v>247</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -9740,7 +9740,7 @@
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>512</v>
       </c>
@@ -9757,7 +9757,7 @@
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>513</v>
       </c>
@@ -9772,7 +9772,7 @@
         <v>248</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -9780,84 +9780,84 @@
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
     </row>
   </sheetData>
@@ -9871,23 +9871,23 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9916,7 +9916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>514</v>
       </c>
@@ -9929,7 +9929,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>515</v>
       </c>
@@ -9941,7 +9941,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>516</v>
       </c>
@@ -9951,7 +9951,7 @@
       <c r="E4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>517</v>
       </c>
@@ -9961,7 +9961,7 @@
       <c r="E5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>518</v>
       </c>
@@ -9973,13 +9973,13 @@
         <v>196</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>519</v>
       </c>
@@ -9989,7 +9989,7 @@
       <c r="E7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>520</v>
       </c>
@@ -9999,7 +9999,7 @@
       <c r="E8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>521</v>
       </c>
@@ -10011,10 +10011,10 @@
         <v>542</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>522</v>
       </c>
@@ -10030,7 +10030,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>523</v>
       </c>
@@ -10043,10 +10043,10 @@
         <v>203</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>544</v>
       </c>
@@ -10062,10 +10062,10 @@
         <v>524</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>525</v>
       </c>
@@ -10076,7 +10076,7 @@
       <c r="E13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>526</v>
       </c>
@@ -10088,11 +10088,11 @@
         <v>201</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>578</v>
+        <v>206</v>
       </c>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>527</v>
       </c>
@@ -10105,76 +10105,76 @@
       <c r="E15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="E16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
     </row>
   </sheetData>
@@ -10187,23 +10187,23 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="179.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="179.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="20.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10232,7 +10232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18.8" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>556</v>
       </c>
@@ -10250,7 +10250,7 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>557</v>
       </c>
@@ -10265,7 +10265,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>558</v>
       </c>
@@ -10274,10 +10274,10 @@
       </c>
       <c r="E4" s="5"/>
       <c r="H4" s="5" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>559</v>
       </c>
@@ -10287,7 +10287,7 @@
       <c r="E5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>560</v>
       </c>
@@ -10302,10 +10302,10 @@
         <v>251</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>561</v>
       </c>
@@ -10317,10 +10317,10 @@
         <v>252</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>566</v>
       </c>
@@ -10329,10 +10329,10 @@
       </c>
       <c r="E8" s="5"/>
       <c r="H8" s="5" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>562</v>
       </c>
@@ -10342,7 +10342,7 @@
       <c r="E9" s="5"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>563</v>
       </c>
@@ -10352,7 +10352,7 @@
       <c r="E10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>564</v>
       </c>
@@ -10362,7 +10362,7 @@
       <c r="E11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>565</v>
       </c>
@@ -10376,16 +10376,16 @@
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H16" s="5"/>
     </row>
   </sheetData>
@@ -10395,12 +10395,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10562,15 +10559,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9BC95A6-9D68-4876-B344-5C0E9EA310F9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17C3FE88-FD63-422B-A211-481C065C3BEF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="a1bb4200-479c-4a05-afd7-28ce53bfa9b9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10594,17 +10602,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17C3FE88-FD63-422B-A211-481C065C3BEF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9BC95A6-9D68-4876-B344-5C0E9EA310F9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a1bb4200-479c-4a05-afd7-28ce53bfa9b9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>